<commit_message>
Deriving datatypes supports 0 of KC (utf8) and 0 of KG (binary) Add separate APIs for using derived datatypes with arrays (debugging) and tables (debugging, parquet, arrow files, arrow streams)
</commit_message>
<xml_diff>
--- a/datatype_layout.xlsx
+++ b/datatype_layout.xlsx
@@ -1,28 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\arrowkdb\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F85A6EB-C000-4FB0-B810-1AC48C030197}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="22995" windowHeight="7995"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="181029"/>
   <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Neal</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -60,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -98,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -136,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0">
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -174,7 +180,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0">
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -212,7 +218,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="0">
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -254,7 +260,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0">
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -296,7 +302,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I3" authorId="0">
+    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -339,7 +345,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J3" authorId="0">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -384,7 +390,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K3" authorId="0">
+    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -453,7 +459,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="0">
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -506,7 +512,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -567,7 +573,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="0">
+    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -633,30 +639,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="M5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Neal:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -814,7 +796,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -916,25 +898,25 @@
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -961,6 +943,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1009,7 +994,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1042,9 +1027,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1077,6 +1079,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1252,12 +1271,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L17" sqref="L17"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1331,138 +1350,138 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="9" t="s">
+      <c r="N3" s="9"/>
+      <c r="O3" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="2"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="9"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="4">
         <v>7</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="5">
         <v>9</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="5">
         <v>14</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="5">
         <v>0</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="5">
         <v>0</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="5">
         <v>0</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="5">
         <v>12</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="5">
         <v>0</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="5">
         <v>0</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="5">
         <v>0</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="5">
         <v>0</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="10">
         <v>0</v>
       </c>
-      <c r="N4" s="12"/>
+      <c r="N4" s="11"/>
       <c r="O4" s="13">
         <v>0</v>
       </c>
       <c r="P4" s="13"/>
-      <c r="Q4" s="12"/>
+      <c r="Q4" s="11"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7">
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5">
         <v>10</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="5">
         <v>4</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="5">
         <v>4</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7">
+      <c r="H5" s="5"/>
+      <c r="I5" s="5">
         <v>4</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="5">
         <v>7</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="5">
         <v>7</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M5" s="6">
         <v>7</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="4">
         <v>9</v>
       </c>
-      <c r="O5" s="8">
+      <c r="O5" s="6">
         <v>5</v>
       </c>
-      <c r="P5" s="10">
+      <c r="P5" s="7">
         <v>7</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q5" s="4">
         <v>9</v>
       </c>
     </row>
@@ -1470,166 +1489,166 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="4">
         <v>1</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="6">
         <v>1</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O6" s="8">
+      <c r="O6" s="6">
         <v>0</v>
       </c>
-      <c r="P6" s="10">
+      <c r="P6" s="7">
         <v>1</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="Q6" s="4">
         <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="6">
+      <c r="B7" s="4">
         <v>2</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="5">
         <v>1.2</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7" s="6">
         <v>2</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="O7" s="8">
+      <c r="O7" s="6">
         <v>1</v>
       </c>
-      <c r="P7" s="10">
+      <c r="P7" s="7">
         <v>2</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q7" s="4">
         <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="6">
+      <c r="B8" s="4">
         <v>3</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="5">
         <v>1.3</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="K8" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="L8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="M8" s="8">
+      <c r="M8" s="6">
         <v>3</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="4">
         <v>3.3</v>
       </c>
-      <c r="O8" s="8">
+      <c r="O8" s="6">
         <v>0</v>
       </c>
-      <c r="P8" s="10">
+      <c r="P8" s="7">
         <v>3</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="Q8" s="4">
         <v>3.3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="O4:Q4"/>
     <mergeCell ref="B1:F2"/>
     <mergeCell ref="G1:I2"/>
     <mergeCell ref="J1:K2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:Q2"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="O4:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1638,7 +1657,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1650,7 +1669,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>